<commit_message>
Spell: obsidian construct - mana tap
</commit_message>
<xml_diff>
--- a/dev/BugTrack.xlsx
+++ b/dev/BugTrack.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="113">
   <si>
     <t>R</t>
   </si>
@@ -357,12 +357,18 @@
   </si>
   <si>
     <t>2015/10/17: 开启英勇打击的情况下死亡会导致永久降低攻击速度</t>
+  </si>
+  <si>
+    <t>反射</t>
+  </si>
+  <si>
+    <t>防骑Q技能对黑曜石雕像</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy&quot;/&quot;mm&quot;/&quot;dd"/>
   </numFmts>
@@ -481,11 +487,53 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="好" xfId="1" builtinId="26"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="适中" xfId="2" builtinId="28"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -542,7 +590,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -617,6 +665,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -652,6 +717,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -805,11 +887,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,45 +941,41 @@
         <v>1</v>
       </c>
       <c r="B2" s="8">
-        <v>41805</v>
+        <v>42703</v>
       </c>
       <c r="C2" s="8"/>
-      <c r="D2" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>42004</v>
-      </c>
-      <c r="C3" s="2">
-        <v>42275</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>41805</v>
+      </c>
+      <c r="C3" s="8"/>
       <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="7"/>
@@ -907,119 +985,115 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>42035</v>
+        <v>42004</v>
       </c>
       <c r="C4" s="2">
-        <v>42036</v>
+        <v>42275</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>18</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
-        <v>3</v>
-      </c>
-      <c r="B5" s="10">
-        <v>41944</v>
-      </c>
-      <c r="C5" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>42035</v>
+      </c>
+      <c r="C5" s="2">
+        <v>42036</v>
+      </c>
       <c r="D5" s="7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="I5" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <v>41840</v>
-      </c>
-      <c r="C6" s="2">
-        <v>41840</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B6" s="10">
+        <v>41944</v>
+      </c>
+      <c r="C6" s="10"/>
       <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>24</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="H6" s="9"/>
       <c r="I6" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2">
         <v>41840</v>
       </c>
       <c r="C7" s="2">
-        <v>41945</v>
+        <v>41840</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>3</v>
       </c>
       <c r="B8" s="2">
-        <v>41839</v>
+        <v>41840</v>
       </c>
       <c r="C8" s="2">
         <v>41945</v>
@@ -1031,12 +1105,14 @@
         <v>19</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="I8" s="7" t="s">
         <v>18</v>
       </c>
@@ -1045,106 +1121,104 @@
       <c r="A9" s="7">
         <v>3</v>
       </c>
-      <c r="B9" s="10">
-        <v>41834</v>
-      </c>
-      <c r="C9" s="10"/>
+      <c r="B9" s="2">
+        <v>41839</v>
+      </c>
+      <c r="C9" s="2">
+        <v>41945</v>
+      </c>
       <c r="D9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>41831</v>
-      </c>
-      <c r="C10" s="1">
-        <v>41840</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B10" s="10">
+        <v>41834</v>
+      </c>
+      <c r="C10" s="10"/>
       <c r="D10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>36</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="H10" s="9"/>
       <c r="I10" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
-        <v>1</v>
-      </c>
-      <c r="B11" s="11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
         <v>41831</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="1">
+        <v>41840</v>
+      </c>
       <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="I11" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>41805</v>
-      </c>
-      <c r="C12" s="1">
-        <v>41840</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B12" s="11">
+        <v>41831</v>
+      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>41</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="H12" s="9"/>
       <c r="I12" s="7" t="s">
         <v>18</v>
       </c>
@@ -1166,21 +1240,21 @@
         <v>10</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1">
         <v>41805</v>
@@ -1192,24 +1266,24 @@
         <v>9</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1">
         <v>41805</v>
@@ -1227,10 +1301,10 @@
         <v>45</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>18</v>
@@ -1253,7 +1327,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>48</v>
@@ -1267,7 +1341,7 @@
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1">
         <v>41805</v>
@@ -1279,22 +1353,22 @@
         <v>9</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>1</v>
       </c>
@@ -1302,22 +1376,22 @@
         <v>41805</v>
       </c>
       <c r="C18" s="1">
-        <v>41839</v>
+        <v>41840</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>18</v>
@@ -1325,30 +1399,34 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="1">
-        <v>41609</v>
+        <v>41805</v>
       </c>
       <c r="C19" s="1">
-        <v>41615</v>
+        <v>41839</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>2</v>
       </c>
@@ -1365,15 +1443,15 @@
         <v>50</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>2</v>
       </c>
@@ -1390,10 +1468,10 @@
         <v>50</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="7"/>
@@ -1415,10 +1493,10 @@
         <v>50</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="7"/>
@@ -1440,17 +1518,17 @@
         <v>50</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1">
         <v>41609</v>
@@ -1462,13 +1540,13 @@
         <v>58</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="7"/>
@@ -1490,17 +1568,17 @@
         <v>69</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26" s="1">
         <v>41609</v>
@@ -1512,18 +1590,18 @@
         <v>58</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>2</v>
       </c>
@@ -1543,12 +1621,12 @@
         <v>39</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>2</v>
       </c>
@@ -1568,14 +1646,14 @@
         <v>39</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29" s="1">
         <v>41609</v>
@@ -1590,10 +1668,10 @@
         <v>30</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="7"/>
@@ -1618,14 +1696,14 @@
         <v>76</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B31" s="1">
         <v>41609</v>
@@ -1643,12 +1721,12 @@
         <v>76</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>2</v>
       </c>
@@ -1668,14 +1746,14 @@
         <v>76</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B33" s="1">
         <v>41609</v>
@@ -1690,10 +1768,10 @@
         <v>30</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="7"/>
@@ -1718,7 +1796,7 @@
         <v>81</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="7"/>
@@ -1743,7 +1821,7 @@
         <v>81</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="7"/>
@@ -1768,7 +1846,7 @@
         <v>81</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="7"/>
@@ -1793,7 +1871,7 @@
         <v>81</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="7"/>
@@ -1818,7 +1896,7 @@
         <v>81</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="7"/>
@@ -1843,7 +1921,7 @@
         <v>81</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="7"/>
@@ -1868,7 +1946,7 @@
         <v>81</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="7"/>
@@ -1890,10 +1968,10 @@
         <v>30</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="7"/>
@@ -1918,14 +1996,14 @@
         <v>90</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B43" s="1">
         <v>41609</v>
@@ -1943,14 +2021,14 @@
         <v>90</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H43" s="9"/>
       <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B44" s="1">
         <v>41609</v>
@@ -1965,17 +2043,17 @@
         <v>30</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B45" s="1">
         <v>41609</v>
@@ -1990,17 +2068,17 @@
         <v>30</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H45" s="9"/>
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B46" s="1">
         <v>41609</v>
@@ -2015,17 +2093,17 @@
         <v>30</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B47" s="1">
         <v>41609</v>
@@ -2037,20 +2115,20 @@
         <v>58</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B48" s="1">
         <v>41609</v>
@@ -2062,20 +2140,20 @@
         <v>58</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H48" s="9"/>
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B49" s="1">
         <v>41609</v>
@@ -2087,13 +2165,13 @@
         <v>58</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>104</v>
+        <v>39</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H49" s="9"/>
       <c r="I49" s="7"/>
@@ -2115,10 +2193,10 @@
         <v>14</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H50" s="9"/>
       <c r="I50" s="7"/>
@@ -2140,28 +2218,68 @@
         <v>14</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H51" s="9"/>
       <c r="I51" s="7"/>
     </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>1</v>
+      </c>
+      <c r="B52" s="1">
+        <v>41609</v>
+      </c>
+      <c r="C52" s="1">
+        <v>41615</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H52" s="9"/>
+      <c r="I52" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A51">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="1">
+  <conditionalFormatting sqref="A1 A3:A52">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH(("1"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A51">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="2">
+  <conditionalFormatting sqref="A1 A3:A52">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH(("2"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A51">
+  <conditionalFormatting sqref="A1 A3:A52">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="3">
+      <formula>NOT(ISERROR(SEARCH(("3"),(A1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH(("1"),(A2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="2">
+      <formula>NOT(ISERROR(SEARCH(("2"),(A2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="3">
-      <formula>NOT(ISERROR(SEARCH(("3"),(A1))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("3"),(A2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>